<commit_message>
updated mysql database with the question bank
</commit_message>
<xml_diff>
--- a/Database/QuizQns.xlsx
+++ b/Database/QuizQns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zihui/Documents/GitHub/DIP-Group-6-Android/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA07D0C-5043-6D47-AD02-DCA3619C5F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7934BC-3B8E-444A-9E0C-EC7EDFDC2BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{90FED666-7C02-AF49-89A4-5692DF621751}"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{90FED666-7C02-AF49-89A4-5692DF621751}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="72">
   <si>
     <t>qnId</t>
   </si>
@@ -161,6 +161,96 @@
   </si>
   <si>
     <t>priId</t>
+  </si>
+  <si>
+    <t>I appreciate hugs or cuddles more than long and sweet messages</t>
+  </si>
+  <si>
+    <t>LoveTest</t>
+  </si>
+  <si>
+    <t>Physical Touch</t>
+  </si>
+  <si>
+    <t>Words of Affirmation</t>
+  </si>
+  <si>
+    <t>I appreciate holding hands than being complimented by the person I like</t>
+  </si>
+  <si>
+    <t>I would rather stay at home and cuddle with my partner than sending motivational messages to my partner</t>
+  </si>
+  <si>
+    <t>I like putting my arms around my partner more than encouraging her verbally</t>
+  </si>
+  <si>
+    <t>I would rather go on a hike with my partner than helping him/her with his/her project</t>
+  </si>
+  <si>
+    <t>I prefer having heart-to-heart talks with my partner to helping him/her for his/her exams</t>
+  </si>
+  <si>
+    <t>I prefer being alone with my partner to helping him/her do the dishes</t>
+  </si>
+  <si>
+    <t>I appreciate having dinner alone with my partner more than fetching him/her from work/school</t>
+  </si>
+  <si>
+    <t>I would rather hug my partner than spend alone time with my partner</t>
+  </si>
+  <si>
+    <t>I would rather encourage my partner when my partner is stressed than help her out</t>
+  </si>
+  <si>
+    <t>Quality Time</t>
+  </si>
+  <si>
+    <t>Act of Service</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>I prefer working alone than in groups.</t>
+  </si>
+  <si>
+    <t>I enjoy meeting clients.</t>
+  </si>
+  <si>
+    <t>I prefer my supervisors to be honest regarding my performances.</t>
+  </si>
+  <si>
+    <t>I prefer to work in a traditional company than a start up.</t>
+  </si>
+  <si>
+    <t>I enjoy attaining physical meetings and conference rather than virtual ones.</t>
+  </si>
+  <si>
+    <t>I prefer my colleagues to not interfere with my personal life.</t>
+  </si>
+  <si>
+    <t>I prefer companies that allows me to share personal opinions and gives room for progression.</t>
+  </si>
+  <si>
+    <t>I prefer working in a community rather than a hierarchical environment.</t>
+  </si>
+  <si>
+    <t>I think everyone is equal without having my boss to tell me so.</t>
+  </si>
+  <si>
+    <t>I do not like my boss to point out my flaws infront of everyone.</t>
+  </si>
+  <si>
+    <t>Outgoing</t>
+  </si>
+  <si>
+    <t>Asocial</t>
+  </si>
+  <si>
+    <t>Idealistic</t>
+  </si>
+  <si>
+    <t>Realistic</t>
   </si>
 </sst>
 </file>
@@ -519,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E462631-6A5C-204A-8FA5-917D9EC6E191}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1551,6 +1641,806 @@
         <v>40</v>
       </c>
     </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>3</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>6</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>6</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>8</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>8</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>9</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>9</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>10</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>10</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>3</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>4</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>5</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>5</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>6</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>6</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>7</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>7</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>8</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>8</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>9</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>9</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>10</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>10</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>